<commit_message>
close to the alpha version
</commit_message>
<xml_diff>
--- a/docu/Q & A/Q&A.xlsx
+++ b/docu/Q & A/Q&A.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22528"/>
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="0" documentId="11_8742E24EE9A3EA1C1248B8ACA613D74B3E9C1A49" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Question</t>
   </si>
@@ -43,6 +43,42 @@
   </si>
   <si>
     <t xml:space="preserve">The output of their model should be the prediction of the building’s representative temperature (volume-averagetemperature of all zones) for the next hour." so I realize, from reading "Report_v2.pdf" that I would "Plans_TwinHouses.pdf”, but I don't have that file. Couldn't you make the representative temperature? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The volumes representing each zone have been added to the "Discription.pdf" Page 5. these values were used as weights to calculate the representative temperature of the building,                                         For your convinence, the volume-averaged temperature of the zones for both the current timestep and the next time step ( namely the output of the models) are added to columns L &amp; M of the file" Twin_house_O5_exp1_60min.xlsx"  respectively </t>
+  </si>
+  <si>
+    <t>"Twin_house_O5_exp1_60min.xlsx"</t>
+  </si>
+  <si>
+    <t>in the "description.pdf" it says : "None of the data for the heat pump and under floor heating provided in the“Twin_house_O5_exp1_60min.xlsx” should not be used for identification purposes" and then later "All the data required for designing the MPC is provided in the file "Twin_house_O5_exp1_60min.xlsx"". So I don't get which data I should use!?</t>
+  </si>
+  <si>
+    <t>This is correct. Data which is in the "Twin-house_O5_exp1_60min.xlsx" should be used for the identification purposes indeed. All that is included in that file is valid for the purpose of this exercise.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Twin-house_O5_exp1_60min.xlsx" </t>
+  </si>
+  <si>
+    <t>Where is u_1 and u_2 in the data? (is it "hp_status_command" and "hp_supply_temp_command" (this one I guess is the actual: "HeatPump_Tsup")?)</t>
+  </si>
+  <si>
+    <t>u1 &amp; u2 are heatpumps status and its supply temperature respectively.  As for the Heat pump's supply temperature there are two columns in the data which one represnts the command applied to the heat pump(hp_supply_temp_command(u2)) and the other one is what heat pump actually supplies us with (HeatPump_actual_Tsup)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Twin-house_O5_exp1_60min.xlsx"                      "Measurement Channel List.xlsx"</t>
+  </si>
+  <si>
+    <t>As I understand you want a model which predicts the representative air temperature as a function of u_1 (HP on/off) and u_2 (supply temperature). I guess that implies that the flow in the heating circuit is constant? Otherwise I don't think it is possible to make a feasible model (at least not linear).</t>
+  </si>
+  <si>
+    <t>Yes Indeed. The flow in the heating system is constant while the heat pump is on, otherwise its zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If I used the "HeatPump_Tsup" simply as the temperature state of the heaters (the floor basically), then I think that I can make a quite straight forward model, however that will not be a function of u_1 and u_2...</t>
+  </si>
+  <si>
+    <t>As it could be seen in the data, heat pump is capable of tracking the supply water command which is given to it quite well so basically there is not much difference between the actual supply temperature and its correspondig command</t>
   </si>
 </sst>
 </file>
@@ -78,9 +114,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -363,11 +405,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -375,7 +417,7 @@
     <col min="1" max="1" width="96.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="45.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
@@ -393,9 +435,56 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="60">
-      <c r="A10" s="1" t="s">
+    <row r="2" spans="1:4" ht="150">
+      <c r="A2" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3">
+        <v>43865</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="75">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="120">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60.75" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="90">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>